<commit_message>
Using added to stream variables, EmptyTest and CustomStringTest properties added. New tests added testing exception throwing and finding sheet by name.
</commit_message>
<xml_diff>
--- a/ExceLite.Unit.Tests/ExcelFiles/MultiLineDate.xlsx
+++ b/ExceLite.Unit.Tests/ExcelFiles/MultiLineDate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerezd\Projektek\ExceLite\ExceLite.Unit.Tests\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7B23E1-2F3D-465B-9EF8-6E0522037FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971122E4-2BA0-4FEE-90A1-C3B204886DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="3825" windowWidth="14985" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>EmptyTest</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>99999.999</t>
+  </si>
+  <si>
+    <t>Custom string property name</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit.</t>
+  </si>
+  <si>
+    <t>Sed do eiusmod tempor incididunt ut labore et dolore.</t>
+  </si>
+  <si>
+    <t>Ut enim ad minim veniam, quis nostrud exercitation.</t>
   </si>
 </sst>
 </file>
@@ -414,18 +426,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,8 +466,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -467,8 +489,11 @@
       <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
@@ -487,8 +512,11 @@
       <c r="G3">
         <v>1000</v>
       </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
@@ -506,6 +534,9 @@
       </c>
       <c r="G4" t="s">
         <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>